<commit_message>
Updated court select spreadsheet and added questions that use it for county and town.
</commit_message>
<xml_diff>
--- a/docassemble/FeewaiverappTestingCourtIntegration/data/sources/ptlacourtaddresstest.xlsx
+++ b/docassemble/FeewaiverappTestingCourtIntegration/data/sources/ptlacourtaddresstest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haycockj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5794F74-C7DD-4BF8-8AB1-B01E3897A914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAE39F6-0061-4630-84DA-AAAAC6AEA845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F67B3C5-B6C4-4449-99CD-A26B95560BC3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="93">
   <si>
     <t>court_code</t>
   </si>
@@ -47,9 +47,6 @@
     <t>department</t>
   </si>
   <si>
-    <t>sddress_county</t>
-  </si>
-  <si>
     <t>Bangor</t>
   </si>
   <si>
@@ -72,6 +69,252 @@
   </si>
   <si>
     <t>Cumberland</t>
+  </si>
+  <si>
+    <t>address_county</t>
+  </si>
+  <si>
+    <t>address_town</t>
+  </si>
+  <si>
+    <t>Portland District Court</t>
+  </si>
+  <si>
+    <t>Augusta District Court</t>
+  </si>
+  <si>
+    <t>Bangor District Court</t>
+  </si>
+  <si>
+    <t>Lewiston District Court</t>
+  </si>
+  <si>
+    <t>Androscoggin</t>
+  </si>
+  <si>
+    <t>Lewiston</t>
+  </si>
+  <si>
+    <t>Belfast District Court</t>
+  </si>
+  <si>
+    <t>Waldo</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Biddeford District Court</t>
+  </si>
+  <si>
+    <t>York</t>
+  </si>
+  <si>
+    <t>Biddeford</t>
+  </si>
+  <si>
+    <t>Bridgton District Court</t>
+  </si>
+  <si>
+    <t>Bridgton</t>
+  </si>
+  <si>
+    <t>Caribou</t>
+  </si>
+  <si>
+    <t>Dover-Foxcroft</t>
+  </si>
+  <si>
+    <t>Ellsworth</t>
+  </si>
+  <si>
+    <t>Farmington</t>
+  </si>
+  <si>
+    <t>Houlton</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Machias</t>
+  </si>
+  <si>
+    <t>Madawaska</t>
+  </si>
+  <si>
+    <t>Millinocket</t>
+  </si>
+  <si>
+    <t>Newport</t>
+  </si>
+  <si>
+    <t>Presque Isle</t>
+  </si>
+  <si>
+    <t>Rockland</t>
+  </si>
+  <si>
+    <t>Rumford</t>
+  </si>
+  <si>
+    <t>Skowhegan</t>
+  </si>
+  <si>
+    <t>South Paris</t>
+  </si>
+  <si>
+    <t>Waterville</t>
+  </si>
+  <si>
+    <t>West Bath</t>
+  </si>
+  <si>
+    <t>Wiscasset</t>
+  </si>
+  <si>
+    <t>Calais</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Aroostook</t>
+  </si>
+  <si>
+    <t>Hancock</t>
+  </si>
+  <si>
+    <t>Piscataquis</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Knox</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Somerset</t>
+  </si>
+  <si>
+    <t>Sagadahoc</t>
+  </si>
+  <si>
+    <t>Calais District Court</t>
+  </si>
+  <si>
+    <t>Caribou District Court</t>
+  </si>
+  <si>
+    <t>Dover-Foxcroft District Court</t>
+  </si>
+  <si>
+    <t>Ellsworth District Court</t>
+  </si>
+  <si>
+    <t>Farmington District Court</t>
+  </si>
+  <si>
+    <t>Houlton District Court</t>
+  </si>
+  <si>
+    <t>Lincoln District Court</t>
+  </si>
+  <si>
+    <t>Machias District Court</t>
+  </si>
+  <si>
+    <t>Madawaska District Court</t>
+  </si>
+  <si>
+    <t>Millinocket District Court</t>
+  </si>
+  <si>
+    <t>Newport District Court</t>
+  </si>
+  <si>
+    <t>Presque Isle District Court</t>
+  </si>
+  <si>
+    <t>Rockland District Court</t>
+  </si>
+  <si>
+    <t>Rumford District Court</t>
+  </si>
+  <si>
+    <t>Skowhegan District Court</t>
+  </si>
+  <si>
+    <t>South Paris District Court</t>
+  </si>
+  <si>
+    <t>Waterville District Court</t>
+  </si>
+  <si>
+    <t>West Bath District Court</t>
+  </si>
+  <si>
+    <t>Wiscasset District Court</t>
+  </si>
+  <si>
+    <t>Penobscot County Superior Court</t>
+  </si>
+  <si>
+    <t>Kennebec County Superior Court</t>
+  </si>
+  <si>
+    <t>Sagadahoc County Superior Court</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>Waldo County Superior Court</t>
+  </si>
+  <si>
+    <t>Aroostook County Superior Court - Caribou</t>
+  </si>
+  <si>
+    <t>Aroostook County Superior Court - Houlton</t>
+  </si>
+  <si>
+    <t>Piscataquis County Superior Court</t>
+  </si>
+  <si>
+    <t>Hancock County Superior Court</t>
+  </si>
+  <si>
+    <t>Franklin County Superior Court</t>
+  </si>
+  <si>
+    <t>Cumberland County Superior Court</t>
+  </si>
+  <si>
+    <t>Oxford County Superior Court</t>
+  </si>
+  <si>
+    <t>Somerset County Superior Court</t>
+  </si>
+  <si>
+    <t>Lincoln County Superior Court</t>
+  </si>
+  <si>
+    <t>Washington County Superior Court</t>
+  </si>
+  <si>
+    <t>Knox County Superior Court</t>
+  </si>
+  <si>
+    <t>Androscoggin County Superior Court</t>
+  </si>
+  <si>
+    <t>Auburn</t>
+  </si>
+  <si>
+    <t>York County Superior Court</t>
   </si>
 </sst>
 </file>
@@ -423,15 +666,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F783C8D-62EB-4557-8712-5AC669CA3EB7}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,63 +692,741 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>